<commit_message>
Yuv i420 to nv12 and rotate 270 in one. 1920*1080, 20ms
</commit_message>
<xml_diff>
--- a/tools/uv-工作簿1.xlsx
+++ b/tools/uv-工作簿1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\AndroidProjects\CCShareHello\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndroidProjects\CCShareHello\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64928A3-32D0-4AF9-ADB0-5B0ADC1AC6A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 -copy (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="126">
   <si>
     <t>U0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -304,14 +304,238 @@
   </si>
   <si>
     <t>v5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>width</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u0'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u1'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u2'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u3'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u5'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u + v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v0'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v5'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u6'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u7'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v6'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v7'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u_height</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +563,15 @@
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,7 +625,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -417,6 +650,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -435,6 +671,72 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D35AFBB-3BAC-4769-8E44-4465A2CFB56D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1816100" y="4686300"/>
+          <a:ext cx="3333750" cy="6534150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -762,19 +1064,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+      <selection activeCell="AF41" sqref="AF41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="32" width="4.1640625" customWidth="1"/>
+    <col min="1" max="34" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -807,8 +1109,10 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
-    </row>
-    <row r="2" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -841,8 +1145,10 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -889,44 +1195,46 @@
       <c r="R3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="1"/>
+      <c r="T3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -969,8 +1277,10 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -1013,8 +1323,10 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1057,8 +1369,10 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1091,8 +1405,2078 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>3</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
+        <v>2</v>
+      </c>
+      <c r="V8" s="3">
+        <v>3</v>
+      </c>
+      <c r="W8" s="3">
+        <v>4</v>
+      </c>
+      <c r="X8" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7">
+        <v>2</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="7">
+        <v>3</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" t="s">
+        <v>33</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="T23" t="s">
+        <v>71</v>
+      </c>
+      <c r="U23" t="s">
+        <v>72</v>
+      </c>
+      <c r="W23" t="s">
+        <v>125</v>
+      </c>
+      <c r="X23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" t="s">
+        <v>70</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>3</v>
+      </c>
+      <c r="X24">
+        <v>6</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA24">
+        <f>(W24 - U24 -1)*2</f>
+        <v>4</v>
+      </c>
+      <c r="AB24">
+        <f>T24</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" t="s">
+        <v>75</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>3</v>
+      </c>
+      <c r="X25">
+        <v>6</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA25">
+        <f>(W25 - U25 -1)*2</f>
+        <v>4</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" ref="AB25:AB34" si="0">T25</f>
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" t="s">
+        <v>77</v>
+      </c>
+      <c r="T26">
+        <v>2</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>3</v>
+      </c>
+      <c r="X26">
+        <v>6</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" ref="AA25:AA34" si="1">(W26 - U26 -1)*2</f>
+        <v>4</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" t="s">
+        <v>82</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>3</v>
+      </c>
+      <c r="X28">
+        <v>6</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+    </row>
+    <row r="29" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" t="s">
+        <v>83</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <v>6</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+    </row>
+    <row r="30" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" t="s">
+        <v>84</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>3</v>
+      </c>
+      <c r="X30">
+        <v>6</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+    </row>
+    <row r="31" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S32" t="s">
+        <v>101</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+      <c r="W32">
+        <v>3</v>
+      </c>
+      <c r="X32">
+        <v>6</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="19:28" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S33" t="s">
+        <v>102</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>2</v>
+      </c>
+      <c r="W33">
+        <v>3</v>
+      </c>
+      <c r="X33">
+        <v>6</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="19:28" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S34" t="s">
+        <v>103</v>
+      </c>
+      <c r="T34">
+        <v>2</v>
+      </c>
+      <c r="U34">
+        <v>2</v>
+      </c>
+      <c r="W34">
+        <v>3</v>
+      </c>
+      <c r="X34">
+        <v>6</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S36" t="s">
+        <v>88</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>3</v>
+      </c>
+      <c r="X36">
+        <v>6</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA36">
+        <f>(W36 - U36-1)*2+1</f>
+        <v>5</v>
+      </c>
+      <c r="AB36">
+        <f>T36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S37" t="s">
+        <v>89</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>3</v>
+      </c>
+      <c r="X37">
+        <v>6</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" ref="AA37:AA46" si="2">(W37 - U37-1)*2+1</f>
+        <v>5</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" ref="AB37:AB46" si="3">T37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S38" t="s">
+        <v>90</v>
+      </c>
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>3</v>
+      </c>
+      <c r="X38">
+        <v>6</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S40" t="s">
+        <v>96</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>3</v>
+      </c>
+      <c r="X40">
+        <v>6</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S41" t="s">
+        <v>97</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>3</v>
+      </c>
+      <c r="X41">
+        <v>6</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S42" t="s">
+        <v>98</v>
+      </c>
+      <c r="T42">
+        <v>2</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <v>3</v>
+      </c>
+      <c r="X42">
+        <v>6</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S44" t="s">
+        <v>107</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>2</v>
+      </c>
+      <c r="W44">
+        <v>3</v>
+      </c>
+      <c r="X44">
+        <v>6</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S45" t="s">
+        <v>108</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>2</v>
+      </c>
+      <c r="W45">
+        <v>3</v>
+      </c>
+      <c r="X45">
+        <v>6</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB45">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="19:28" x14ac:dyDescent="0.3">
+      <c r="S46" t="s">
+        <v>109</v>
+      </c>
+      <c r="T46">
+        <v>2</v>
+      </c>
+      <c r="U46">
+        <v>2</v>
+      </c>
+      <c r="W46">
+        <v>3</v>
+      </c>
+      <c r="X46">
+        <v>6</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="S52" s="8">
+        <v>0</v>
+      </c>
+      <c r="T52" s="8">
+        <v>1</v>
+      </c>
+      <c r="U52" s="8">
+        <v>2</v>
+      </c>
+      <c r="V52" s="8">
+        <v>3</v>
+      </c>
+      <c r="W52" s="8">
+        <v>4</v>
+      </c>
+      <c r="X52" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K53" t="s">
+        <v>26</v>
+      </c>
+      <c r="L53" t="s">
+        <v>20</v>
+      </c>
+      <c r="S53" t="s">
+        <v>32</v>
+      </c>
+      <c r="T53" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" t="s">
+        <v>26</v>
+      </c>
+      <c r="V53" t="s">
+        <v>27</v>
+      </c>
+      <c r="W53" t="s">
+        <v>20</v>
+      </c>
+      <c r="X53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54" t="s">
+        <v>22</v>
+      </c>
+      <c r="S54" t="s">
+        <v>34</v>
+      </c>
+      <c r="T54" t="s">
+        <v>35</v>
+      </c>
+      <c r="U54" t="s">
+        <v>28</v>
+      </c>
+      <c r="V54" t="s">
+        <v>29</v>
+      </c>
+      <c r="W54" t="s">
+        <v>22</v>
+      </c>
+      <c r="X54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K55" t="s">
+        <v>30</v>
+      </c>
+      <c r="L55" t="s">
+        <v>24</v>
+      </c>
+      <c r="S55" t="s">
+        <v>36</v>
+      </c>
+      <c r="T55" t="s">
+        <v>37</v>
+      </c>
+      <c r="U55" t="s">
+        <v>30</v>
+      </c>
+      <c r="V55" t="s">
+        <v>31</v>
+      </c>
+      <c r="W55" t="s">
+        <v>24</v>
+      </c>
+      <c r="X55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K56" t="s">
+        <v>27</v>
+      </c>
+      <c r="L56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K57" t="s">
+        <v>29</v>
+      </c>
+      <c r="L57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="11:24" x14ac:dyDescent="0.3">
+      <c r="K58" t="s">
+        <v>31</v>
+      </c>
+      <c r="L58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="33" width="4.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3">
@@ -1157,8 +3541,9 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>0</v>
@@ -1227,8 +3612,9 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>1</v>
@@ -1297,8 +3683,9 @@
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>2</v>
@@ -1367,8 +3754,9 @@
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>3</v>
@@ -1437,8 +3825,9 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
-    </row>
-    <row r="13" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG12" s="1"/>
+    </row>
+    <row r="13" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
@@ -1497,8 +3886,9 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG13" s="1"/>
+    </row>
+    <row r="14" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
@@ -1557,8 +3947,9 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG14" s="1"/>
+    </row>
+    <row r="15" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -1601,8 +3992,9 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG15" s="1"/>
+    </row>
+    <row r="16" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
@@ -1645,8 +4037,9 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG16" s="1"/>
+    </row>
+    <row r="17" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -1683,8 +4076,9 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG17" s="1"/>
+    </row>
+    <row r="18" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
@@ -1721,8 +4115,9 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG18" s="1"/>
+    </row>
+    <row r="19" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
@@ -1759,8 +4154,9 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG19" s="1"/>
+    </row>
+    <row r="20" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -1797,8 +4193,9 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG20" s="1"/>
+    </row>
+    <row r="21" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1831,8 +4228,9 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
-    </row>
-    <row r="22" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG21" s="1"/>
+    </row>
+    <row r="22" spans="1:33" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1865,8 +4263,9 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
-    </row>
-    <row r="23" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG22" s="1"/>
+    </row>
+    <row r="23" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1899,8 +4298,9 @@
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG23" s="1"/>
+    </row>
+    <row r="24" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1933,8 +4333,9 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG24" s="1"/>
+    </row>
+    <row r="25" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1967,8 +4368,9 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
-    </row>
-    <row r="26" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG25" s="1"/>
+    </row>
+    <row r="26" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2001,8 +4403,9 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
-    </row>
-    <row r="27" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG26" s="1"/>
+    </row>
+    <row r="27" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2031,15 +4434,455 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
+      <c r="AC27" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="AG27" s="1"/>
+    </row>
+    <row r="28" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y28" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X29" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>3</v>
+      </c>
+      <c r="AC29">
+        <v>4</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF29">
+        <f>(AC29-Z29-1-1)*2 -2</f>
+        <v>2</v>
+      </c>
+      <c r="AG29">
+        <f>Y29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <v>3</v>
+      </c>
+      <c r="AC30">
+        <v>4</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF30">
+        <f>(AC30-Z30-1-1)*2 -2</f>
+        <v>2</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" ref="AG30:AG43" si="0">Y30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="X31" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y31">
+        <v>2</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>3</v>
+      </c>
+      <c r="AC31">
+        <v>4</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" ref="AF30:AF39" si="1">(AC31-Z31-1-1)*2 -2</f>
+        <v>2</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X33" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>3</v>
+      </c>
+      <c r="AC33">
+        <v>4</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X34" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <v>1</v>
+      </c>
+      <c r="AB34">
+        <v>3</v>
+      </c>
+      <c r="AC34">
+        <v>4</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X35" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y35">
+        <v>2</v>
+      </c>
+      <c r="Z35">
+        <v>1</v>
+      </c>
+      <c r="AB35">
+        <v>3</v>
+      </c>
+      <c r="AC35">
+        <v>4</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X37" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>2</v>
+      </c>
+      <c r="AB37">
+        <v>3</v>
+      </c>
+      <c r="AC37">
+        <v>4</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X38" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+      <c r="Z38">
+        <v>2</v>
+      </c>
+      <c r="AB38">
+        <v>3</v>
+      </c>
+      <c r="AC38">
+        <v>4</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X39" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y39">
+        <v>2</v>
+      </c>
+      <c r="Z39">
+        <v>2</v>
+      </c>
+      <c r="AB39">
+        <v>3</v>
+      </c>
+      <c r="AC39">
+        <v>4</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X41" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>2</v>
+      </c>
+      <c r="AB41">
+        <v>3</v>
+      </c>
+      <c r="AC41">
+        <v>4</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF41">
+        <f>(AC41-Z41)*2-1</f>
+        <v>3</v>
+      </c>
+      <c r="AG41">
+        <f>Y41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X42" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+      <c r="Z42">
+        <v>2</v>
+      </c>
+      <c r="AB42">
+        <v>3</v>
+      </c>
+      <c r="AC42">
+        <v>4</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF42">
+        <f>(AC42-Z42)*2-1</f>
+        <v>3</v>
+      </c>
+      <c r="AG42">
+        <f>Y42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X43" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y43">
+        <v>2</v>
+      </c>
+      <c r="Z43">
+        <v>2</v>
+      </c>
+      <c r="AB43">
+        <v>3</v>
+      </c>
+      <c r="AC43">
+        <v>4</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF43">
+        <f t="shared" ref="AF42:AF47" si="2">(AC43-Z43)*2-1</f>
+        <v>3</v>
+      </c>
+      <c r="AG43">
+        <f>Y43</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X45" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>3</v>
+      </c>
+      <c r="AB45">
+        <v>3</v>
+      </c>
+      <c r="AC45">
+        <v>4</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AG45">
+        <f>Y45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X46" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y46">
+        <v>1</v>
+      </c>
+      <c r="Z46">
+        <v>3</v>
+      </c>
+      <c r="AB46">
+        <v>3</v>
+      </c>
+      <c r="AC46">
+        <v>4</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AG46">
+        <f>Y46</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="24:33" x14ac:dyDescent="0.3">
+      <c r="X47" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y47">
+        <v>2</v>
+      </c>
+      <c r="Z47">
+        <v>3</v>
+      </c>
+      <c r="AB47">
+        <v>3</v>
+      </c>
+      <c r="AC47">
+        <v>4</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF47">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AG47">
+        <f>Y47</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K49" t="s">
         <v>26</v>
       </c>
@@ -2058,8 +4901,14 @@
       <c r="R49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="X49" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K50" t="s">
         <v>28</v>
       </c>
@@ -2078,8 +4927,14 @@
       <c r="R50" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="X50" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K51" t="s">
         <v>30</v>
       </c>
@@ -2098,8 +4953,14 @@
       <c r="R51" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="X51" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K52" t="s">
         <v>27</v>
       </c>
@@ -2107,7 +4968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="11:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K53" t="s">
         <v>29</v>
       </c>
@@ -2115,7 +4976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="11:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="11:25" x14ac:dyDescent="0.3">
       <c r="K54" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
convert a u-block once routine.
</commit_message>
<xml_diff>
--- a/tools/uv-工作簿1.xlsx
+++ b/tools/uv-工作簿1.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 -copy (2)" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="视频尺寸" sheetId="3" r:id="rId3"/>
+    <sheet name="视频-blocks-转换--依据这个转换" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="336">
   <si>
     <t>U0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -528,6 +530,689 @@
   </si>
   <si>
     <t>u_height</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full HD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标清</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流畅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>width/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>height/8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>y6</t>
+  </si>
+  <si>
+    <t>y7</t>
+  </si>
+  <si>
+    <t>y8</t>
+  </si>
+  <si>
+    <t>y9</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>y5</t>
+  </si>
+  <si>
+    <t>y10</t>
+  </si>
+  <si>
+    <t>y11</t>
+  </si>
+  <si>
+    <t>y12</t>
+  </si>
+  <si>
+    <t>y13</t>
+  </si>
+  <si>
+    <t>y14</t>
+  </si>
+  <si>
+    <t>y15</t>
+  </si>
+  <si>
+    <t>y19</t>
+  </si>
+  <si>
+    <t>y20</t>
+  </si>
+  <si>
+    <t>y21</t>
+  </si>
+  <si>
+    <t>y22</t>
+  </si>
+  <si>
+    <t>y23</t>
+  </si>
+  <si>
+    <t>y24</t>
+  </si>
+  <si>
+    <t>y25</t>
+  </si>
+  <si>
+    <t>y26</t>
+  </si>
+  <si>
+    <t>y27</t>
+  </si>
+  <si>
+    <t>y28</t>
+  </si>
+  <si>
+    <t>y29</t>
+  </si>
+  <si>
+    <t>y30</t>
+  </si>
+  <si>
+    <t>y31</t>
+  </si>
+  <si>
+    <t>y34</t>
+  </si>
+  <si>
+    <t>y35</t>
+  </si>
+  <si>
+    <t>y36</t>
+  </si>
+  <si>
+    <t>y37</t>
+  </si>
+  <si>
+    <t>y38</t>
+  </si>
+  <si>
+    <t>y39</t>
+  </si>
+  <si>
+    <t>y40</t>
+  </si>
+  <si>
+    <t>y41</t>
+  </si>
+  <si>
+    <t>y42</t>
+  </si>
+  <si>
+    <t>y43</t>
+  </si>
+  <si>
+    <t>y44</t>
+  </si>
+  <si>
+    <t>y45</t>
+  </si>
+  <si>
+    <t>y46</t>
+  </si>
+  <si>
+    <t>y47</t>
+  </si>
+  <si>
+    <t>y48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y50</t>
+  </si>
+  <si>
+    <t>y51</t>
+  </si>
+  <si>
+    <t>y52</t>
+  </si>
+  <si>
+    <t>y53</t>
+  </si>
+  <si>
+    <t>y54</t>
+  </si>
+  <si>
+    <t>y55</t>
+  </si>
+  <si>
+    <t>y56</t>
+  </si>
+  <si>
+    <t>y57</t>
+  </si>
+  <si>
+    <t>y58</t>
+  </si>
+  <si>
+    <t>y59</t>
+  </si>
+  <si>
+    <t>y60</t>
+  </si>
+  <si>
+    <t>y61</t>
+  </si>
+  <si>
+    <t>y62</t>
+  </si>
+  <si>
+    <t>y63</t>
+  </si>
+  <si>
+    <t>y64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y66</t>
+  </si>
+  <si>
+    <t>y67</t>
+  </si>
+  <si>
+    <t>y65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y66</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y68</t>
+  </si>
+  <si>
+    <t>y69</t>
+  </si>
+  <si>
+    <t>y70</t>
+  </si>
+  <si>
+    <t>y71</t>
+  </si>
+  <si>
+    <t>y72</t>
+  </si>
+  <si>
+    <t>y73</t>
+  </si>
+  <si>
+    <t>y74</t>
+  </si>
+  <si>
+    <t>y75</t>
+  </si>
+  <si>
+    <t>y76</t>
+  </si>
+  <si>
+    <t>y77</t>
+  </si>
+  <si>
+    <t>y78</t>
+  </si>
+  <si>
+    <t>y79</t>
+  </si>
+  <si>
+    <t>y80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y81</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y82</t>
+  </si>
+  <si>
+    <t>y83</t>
+  </si>
+  <si>
+    <t>y84</t>
+  </si>
+  <si>
+    <t>y85</t>
+  </si>
+  <si>
+    <t>y86</t>
+  </si>
+  <si>
+    <t>y87</t>
+  </si>
+  <si>
+    <t>y88</t>
+  </si>
+  <si>
+    <t>y89</t>
+  </si>
+  <si>
+    <t>y90</t>
+  </si>
+  <si>
+    <t>y91</t>
+  </si>
+  <si>
+    <t>y92</t>
+  </si>
+  <si>
+    <t>y93</t>
+  </si>
+  <si>
+    <t>y94</t>
+  </si>
+  <si>
+    <t>y95</t>
+  </si>
+  <si>
+    <t>y96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y97</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y98</t>
+  </si>
+  <si>
+    <t>y99</t>
+  </si>
+  <si>
+    <t>y100</t>
+  </si>
+  <si>
+    <t>y101</t>
+  </si>
+  <si>
+    <t>y102</t>
+  </si>
+  <si>
+    <t>y103</t>
+  </si>
+  <si>
+    <t>y104</t>
+  </si>
+  <si>
+    <t>y105</t>
+  </si>
+  <si>
+    <t>y106</t>
+  </si>
+  <si>
+    <t>y107</t>
+  </si>
+  <si>
+    <t>y108</t>
+  </si>
+  <si>
+    <t>y109</t>
+  </si>
+  <si>
+    <t>y110</t>
+  </si>
+  <si>
+    <t>y111</t>
+  </si>
+  <si>
+    <t>y112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y114</t>
+  </si>
+  <si>
+    <t>y115</t>
+  </si>
+  <si>
+    <t>y116</t>
+  </si>
+  <si>
+    <t>y117</t>
+  </si>
+  <si>
+    <t>y118</t>
+  </si>
+  <si>
+    <t>y119</t>
+  </si>
+  <si>
+    <t>y120</t>
+  </si>
+  <si>
+    <t>y121</t>
+  </si>
+  <si>
+    <t>y122</t>
+  </si>
+  <si>
+    <t>y123</t>
+  </si>
+  <si>
+    <t>y124</t>
+  </si>
+  <si>
+    <t>y125</t>
+  </si>
+  <si>
+    <t>y126</t>
+  </si>
+  <si>
+    <t>y127</t>
+  </si>
+  <si>
+    <t>u3</t>
+  </si>
+  <si>
+    <t>u4</t>
+  </si>
+  <si>
+    <t>u5</t>
+  </si>
+  <si>
+    <t>u6</t>
+  </si>
+  <si>
+    <t>u7</t>
+  </si>
+  <si>
+    <t>u10</t>
+  </si>
+  <si>
+    <t>u11</t>
+  </si>
+  <si>
+    <t>u12</t>
+  </si>
+  <si>
+    <t>u13</t>
+  </si>
+  <si>
+    <t>u14</t>
+  </si>
+  <si>
+    <t>u15</t>
+  </si>
+  <si>
+    <t>u16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u18</t>
+  </si>
+  <si>
+    <t>u19</t>
+  </si>
+  <si>
+    <t>u20</t>
+  </si>
+  <si>
+    <t>u21</t>
+  </si>
+  <si>
+    <t>u22</t>
+  </si>
+  <si>
+    <t>u23</t>
+  </si>
+  <si>
+    <t>u24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u26</t>
+  </si>
+  <si>
+    <t>u27</t>
+  </si>
+  <si>
+    <t>u28</t>
+  </si>
+  <si>
+    <t>u29</t>
+  </si>
+  <si>
+    <t>u30</t>
+  </si>
+  <si>
+    <t>u31</t>
+  </si>
+  <si>
+    <t>u18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t>v10</t>
+  </si>
+  <si>
+    <t>v11</t>
+  </si>
+  <si>
+    <t>v12</t>
+  </si>
+  <si>
+    <t>v13</t>
+  </si>
+  <si>
+    <t>v14</t>
+  </si>
+  <si>
+    <t>v15</t>
+  </si>
+  <si>
+    <t>v16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v18</t>
+  </si>
+  <si>
+    <t>v19</t>
+  </si>
+  <si>
+    <t>v20</t>
+  </si>
+  <si>
+    <t>v21</t>
+  </si>
+  <si>
+    <t>v22</t>
+  </si>
+  <si>
+    <t>v23</t>
+  </si>
+  <si>
+    <t>v24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v26</t>
+  </si>
+  <si>
+    <t>v27</t>
+  </si>
+  <si>
+    <t>v28</t>
+  </si>
+  <si>
+    <t>v29</t>
+  </si>
+  <si>
+    <t>v30</t>
+  </si>
+  <si>
+    <t>v31</t>
+  </si>
+  <si>
+    <t>Rotate right 90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YU12(I420)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详解 YUV 格式（I420/YUV420/NV12/NV12/YUV422） - 掘金 (juejin.cn)</t>
+  </si>
+  <si>
+    <t>NV12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,7 +1220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +1258,72 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -582,7 +1333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -619,13 +1370,480 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -653,12 +1871,282 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -781,6 +2269,357 @@
         <a:xfrm>
           <a:off x="1816100" y="4686300"/>
           <a:ext cx="3333750" cy="6534150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>147447</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="9686227" y="1731073"/>
+          <a:ext cx="4106672" cy="1616075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>119495</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="12319577" y="1224973"/>
+          <a:ext cx="2551545" cy="1016000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4101" name="AutoShape 5" descr="YU12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="311150" y="5778500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4102" name="AutoShape 6" descr="YU12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="311150" y="5778500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="342900" y="5905500"/>
+          <a:ext cx="1841500" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4105" name="AutoShape 9" descr="NV12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8712200" y="6889750"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9055100" y="6705600"/>
+          <a:ext cx="1841500" cy="1104900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1067,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="AF41" sqref="AF41"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2456,7 +4295,7 @@
         <v>78</v>
       </c>
       <c r="AA26">
-        <f t="shared" ref="AA25:AA34" si="1">(W26 - U26 -1)*2</f>
+        <f t="shared" ref="AA26:AA34" si="1">(W26 - U26 -1)*2</f>
         <v>4</v>
       </c>
       <c r="AB26">
@@ -3142,8 +4981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="Z41" sqref="Z41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4514,7 +6353,7 @@
         <v>2</v>
       </c>
       <c r="AG30">
-        <f t="shared" ref="AG30:AG43" si="0">Y30</f>
+        <f t="shared" ref="AG30:AG39" si="0">Y30</f>
         <v>1</v>
       </c>
     </row>
@@ -4538,7 +6377,7 @@
         <v>78</v>
       </c>
       <c r="AF31">
-        <f t="shared" ref="AF30:AF39" si="1">(AC31-Z31-1-1)*2 -2</f>
+        <f t="shared" ref="AF31:AF39" si="1">(AC31-Z31-1-1)*2 -2</f>
         <v>2</v>
       </c>
       <c r="AG31">
@@ -4790,7 +6629,7 @@
         <v>95</v>
       </c>
       <c r="AF43">
-        <f t="shared" ref="AF42:AF47" si="2">(AC43-Z43)*2-1</f>
+        <f t="shared" ref="AF43:AF47" si="2">(AC43-Z43)*2-1</f>
         <v>3</v>
       </c>
       <c r="AG43">
@@ -4990,4 +6829,2266 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>3240</v>
+      </c>
+      <c r="D2">
+        <v>2160</v>
+      </c>
+      <c r="F2">
+        <f>C2/8</f>
+        <v>405</v>
+      </c>
+      <c r="G2">
+        <f>D2/8</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3">
+        <v>2160</v>
+      </c>
+      <c r="D3">
+        <v>1440</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="0">C3/8</f>
+        <v>270</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="1">D3/8</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <v>1920</v>
+      </c>
+      <c r="D4">
+        <v>1080</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5">
+        <v>1280</v>
+      </c>
+      <c r="D5">
+        <v>720</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>640</v>
+      </c>
+      <c r="D6">
+        <v>480</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7">
+        <v>720</v>
+      </c>
+      <c r="D7">
+        <v>480</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8">
+        <v>320</v>
+      </c>
+      <c r="D8">
+        <v>240</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9">
+        <v>720</v>
+      </c>
+      <c r="D9">
+        <v>1280</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AV45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="41" width="4.08203125" customWidth="1"/>
+    <col min="42" max="46" width="4.75" customWidth="1"/>
+    <col min="47" max="51" width="4.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20">
+        <v>3</v>
+      </c>
+      <c r="G2" s="20">
+        <v>4</v>
+      </c>
+      <c r="H2" s="20">
+        <v>5</v>
+      </c>
+      <c r="I2" s="20">
+        <v>6</v>
+      </c>
+      <c r="J2" s="20">
+        <v>7</v>
+      </c>
+      <c r="K2" s="20">
+        <v>8</v>
+      </c>
+      <c r="L2" s="20">
+        <v>9</v>
+      </c>
+      <c r="M2" s="20">
+        <v>10</v>
+      </c>
+      <c r="N2" s="20">
+        <v>11</v>
+      </c>
+      <c r="O2" s="20">
+        <v>12</v>
+      </c>
+      <c r="P2" s="20">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>14</v>
+      </c>
+      <c r="R2" s="20">
+        <v>15</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="U2" s="16">
+        <v>0</v>
+      </c>
+      <c r="V2" s="16">
+        <v>1</v>
+      </c>
+      <c r="W2" s="16">
+        <v>2</v>
+      </c>
+      <c r="X2" s="16">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="16">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="16">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="16">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="14"/>
+      <c r="AP2" t="s">
+        <v>324</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q3" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="R3" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" s="17">
+        <v>0</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z3" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" s="66"/>
+    </row>
+    <row r="4" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="81" t="s">
+        <v>156</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="T4" s="17">
+        <v>1</v>
+      </c>
+      <c r="U4" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="V4" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="W4" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y4" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC4" s="67"/>
+    </row>
+    <row r="5" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="20">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="R5" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="T5" s="17">
+        <v>2</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="W5" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="X5" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC5" s="67"/>
+    </row>
+    <row r="6" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="81" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="R6" s="82" t="s">
+        <v>193</v>
+      </c>
+      <c r="T6" s="17">
+        <v>3</v>
+      </c>
+      <c r="U6" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="W6" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="X6" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA6" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" s="67"/>
+    </row>
+    <row r="7" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="41">
+        <v>4</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="K7" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="R7" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="T7" s="17">
+        <v>4</v>
+      </c>
+      <c r="U7" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="W7" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="X7" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z7" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA7" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="67"/>
+    </row>
+    <row r="8" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41">
+        <v>5</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="R8" s="82" t="s">
+        <v>226</v>
+      </c>
+      <c r="T8" s="17">
+        <v>5</v>
+      </c>
+      <c r="U8" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="V8" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="W8" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="X8" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y8" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z8" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA8" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB8" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC8" s="67"/>
+    </row>
+    <row r="9" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="41">
+        <v>6</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="K9" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="R9" s="82" t="s">
+        <v>242</v>
+      </c>
+      <c r="T9" s="17">
+        <v>6</v>
+      </c>
+      <c r="U9" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="V9" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="W9" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="X9" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y9" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z9" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="67"/>
+    </row>
+    <row r="10" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="41">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="K10" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="L10" s="84" t="s">
+        <v>252</v>
+      </c>
+      <c r="M10" s="84" t="s">
+        <v>253</v>
+      </c>
+      <c r="N10" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="O10" s="84" t="s">
+        <v>255</v>
+      </c>
+      <c r="P10" s="84" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q10" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="R10" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="T10" s="17">
+        <v>7</v>
+      </c>
+      <c r="U10" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="V10" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="W10" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="X10" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y10" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z10" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA10" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC10" s="67"/>
+    </row>
+    <row r="11" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="59"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="58"/>
+      <c r="T11" s="17">
+        <v>8</v>
+      </c>
+      <c r="U11" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="V11" s="79" t="s">
+        <v>235</v>
+      </c>
+      <c r="W11" s="79" t="s">
+        <v>219</v>
+      </c>
+      <c r="X11" s="79" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y11" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z11" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA11" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB11" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC11" s="67"/>
+    </row>
+    <row r="12" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="T12" s="17">
+        <v>9</v>
+      </c>
+      <c r="U12" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="V12" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="W12" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="X12" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y12" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z12" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA12" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB12" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" s="67"/>
+    </row>
+    <row r="13" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>4</v>
+      </c>
+      <c r="H13" s="9">
+        <v>5</v>
+      </c>
+      <c r="I13" s="9">
+        <v>6</v>
+      </c>
+      <c r="J13" s="9">
+        <v>7</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="T13" s="17">
+        <v>10</v>
+      </c>
+      <c r="U13" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="V13" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="W13" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="X13" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y13" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z13" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA13" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB13" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC13" s="67"/>
+    </row>
+    <row r="14" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="18">
+        <v>0</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="H14" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="I14" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="T14" s="17">
+        <v>11</v>
+      </c>
+      <c r="U14" s="81" t="s">
+        <v>254</v>
+      </c>
+      <c r="V14" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="W14" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="X14" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y14" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z14" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA14" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB14" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC14" s="67"/>
+    </row>
+    <row r="15" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>266</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="J15" s="75" t="s">
+        <v>269</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="T15" s="17">
+        <v>12</v>
+      </c>
+      <c r="U15" s="81" t="s">
+        <v>255</v>
+      </c>
+      <c r="V15" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="W15" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="X15" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y15" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z15" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA15" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB15" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC15" s="67"/>
+    </row>
+    <row r="16" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="G16" s="77" t="s">
+        <v>288</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="J16" s="75" t="s">
+        <v>291</v>
+      </c>
+      <c r="T16" s="17">
+        <v>13</v>
+      </c>
+      <c r="U16" s="81" t="s">
+        <v>256</v>
+      </c>
+      <c r="V16" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="W16" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="X16" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y16" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z16" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA16" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB16" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC16" s="67"/>
+    </row>
+    <row r="17" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="18">
+        <v>3</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="H17" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="I17" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="T17" s="17">
+        <v>14</v>
+      </c>
+      <c r="U17" s="81" t="s">
+        <v>257</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="W17" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="X17" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y17" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z17" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA17" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB17" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC17" s="67"/>
+    </row>
+    <row r="18" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="18"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
+      <c r="T18" s="17">
+        <v>15</v>
+      </c>
+      <c r="U18" s="83" t="s">
+        <v>258</v>
+      </c>
+      <c r="V18" s="84" t="s">
+        <v>242</v>
+      </c>
+      <c r="W18" s="84" t="s">
+        <v>226</v>
+      </c>
+      <c r="X18" s="84" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y18" s="84" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z18" s="84" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA18" s="84" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB18" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC18" s="68"/>
+    </row>
+    <row r="19" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AF19" s="19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>3</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4</v>
+      </c>
+      <c r="H20" s="11">
+        <v>5</v>
+      </c>
+      <c r="I20" s="11">
+        <v>6</v>
+      </c>
+      <c r="J20" s="11">
+        <v>7</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="T20" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="U20" s="16">
+        <v>0</v>
+      </c>
+      <c r="V20" s="16">
+        <v>1</v>
+      </c>
+      <c r="W20" s="16">
+        <v>2</v>
+      </c>
+      <c r="X20" s="16">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE20" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="56">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="16">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="56">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="16">
+        <v>2</v>
+      </c>
+      <c r="AJ20" s="56">
+        <v>2</v>
+      </c>
+      <c r="AK20" s="16">
+        <v>3</v>
+      </c>
+      <c r="AL20" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="18">
+        <v>0</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="86" t="s">
+        <v>298</v>
+      </c>
+      <c r="H21" s="87" t="s">
+        <v>299</v>
+      </c>
+      <c r="I21" s="87" t="s">
+        <v>300</v>
+      </c>
+      <c r="J21" s="88" t="s">
+        <v>301</v>
+      </c>
+      <c r="T21" s="17">
+        <v>0</v>
+      </c>
+      <c r="U21" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="V21" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="W21" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y21" s="69"/>
+      <c r="AD21" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="AF21" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="AG21" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="AH21" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="AI21" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ21" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK21" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL21" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM21" s="71"/>
+    </row>
+    <row r="22" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18">
+        <v>1</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="G22" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="J22" s="75" t="s">
+        <v>307</v>
+      </c>
+      <c r="T22" s="17">
+        <v>1</v>
+      </c>
+      <c r="U22" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="V22" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="W22" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="X22" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y22" s="67"/>
+      <c r="AD22" s="17">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="AF22" s="48" t="s">
+        <v>317</v>
+      </c>
+      <c r="AG22" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH22" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="AI22" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ22" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK22" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL22" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM22" s="72"/>
+      <c r="AO22" s="16"/>
+    </row>
+    <row r="23" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18">
+        <v>2</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="G23" s="77" t="s">
+        <v>312</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="J23" s="75" t="s">
+        <v>315</v>
+      </c>
+      <c r="T23" s="17">
+        <v>2</v>
+      </c>
+      <c r="U23" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="V23" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="W23" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="X23" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y23" s="70"/>
+      <c r="AD23" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE23" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF23" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="AG23" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH23" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="AI23" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ23" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="AK23" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL23" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM23" s="72"/>
+      <c r="AO23" s="25"/>
+    </row>
+    <row r="24" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="18">
+        <v>3</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="F24" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="H24" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="T24" s="17">
+        <v>3</v>
+      </c>
+      <c r="U24" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="V24" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="W24" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="X24" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y24" s="70"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="17">
+        <v>3</v>
+      </c>
+      <c r="AE24" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF24" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="AG24" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="AH24" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="AI24" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ24" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="AK24" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL24" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM24" s="72"/>
+      <c r="AO24" s="25"/>
+    </row>
+    <row r="25" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="65"/>
+      <c r="T25" s="17">
+        <v>4</v>
+      </c>
+      <c r="U25" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="V25" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="W25" s="79" t="s">
+        <v>266</v>
+      </c>
+      <c r="X25" s="80" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y25" s="70"/>
+      <c r="AD25" s="17">
+        <v>4</v>
+      </c>
+      <c r="AE25" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="AF25" s="79" t="s">
+        <v>320</v>
+      </c>
+      <c r="AG25" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="AH25" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI25" s="79" t="s">
+        <v>266</v>
+      </c>
+      <c r="AJ25" s="79" t="s">
+        <v>304</v>
+      </c>
+      <c r="AK25" s="79" t="s">
+        <v>260</v>
+      </c>
+      <c r="AL25" s="80" t="s">
+        <v>298</v>
+      </c>
+      <c r="AM25" s="72"/>
+      <c r="AO25" s="25"/>
+    </row>
+    <row r="26" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T26" s="17">
+        <v>5</v>
+      </c>
+      <c r="U26" s="81" t="s">
+        <v>283</v>
+      </c>
+      <c r="V26" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="W26" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="X26" s="82" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y26" s="70"/>
+      <c r="AD26" s="17">
+        <v>5</v>
+      </c>
+      <c r="AE26" s="81" t="s">
+        <v>283</v>
+      </c>
+      <c r="AF26" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="AG26" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH26" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI26" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ26" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK26" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AL26" s="82" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM26" s="72"/>
+      <c r="AO26" s="25"/>
+    </row>
+    <row r="27" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>333</v>
+      </c>
+      <c r="T27" s="17">
+        <v>6</v>
+      </c>
+      <c r="U27" s="81" t="s">
+        <v>284</v>
+      </c>
+      <c r="V27" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="W27" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="X27" s="82" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y27" s="70"/>
+      <c r="AD27" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE27" s="81" t="s">
+        <v>284</v>
+      </c>
+      <c r="AF27" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="AG27" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="AH27" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="AI27" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="AJ27" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="AK27" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AL27" s="82" t="s">
+        <v>300</v>
+      </c>
+      <c r="AM27" s="72"/>
+      <c r="AO27" s="9"/>
+    </row>
+    <row r="28" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="55" t="s">
+        <v>334</v>
+      </c>
+      <c r="T28" s="17">
+        <v>7</v>
+      </c>
+      <c r="U28" s="83" t="s">
+        <v>285</v>
+      </c>
+      <c r="V28" s="84" t="s">
+        <v>277</v>
+      </c>
+      <c r="W28" s="84" t="s">
+        <v>269</v>
+      </c>
+      <c r="X28" s="85" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y28" s="65"/>
+      <c r="AD28" s="17">
+        <v>7</v>
+      </c>
+      <c r="AE28" s="83" t="s">
+        <v>285</v>
+      </c>
+      <c r="AF28" s="94" t="s">
+        <v>323</v>
+      </c>
+      <c r="AG28" s="84" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH28" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="AI28" s="84" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ28" s="94" t="s">
+        <v>307</v>
+      </c>
+      <c r="AK28" s="84" t="s">
+        <v>263</v>
+      </c>
+      <c r="AL28" s="96" t="s">
+        <v>301</v>
+      </c>
+      <c r="AM28" s="73"/>
+      <c r="AO28" s="9"/>
+    </row>
+    <row r="29" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AO29" s="9"/>
+    </row>
+    <row r="30" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T30" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="U30" s="56">
+        <v>0</v>
+      </c>
+      <c r="V30" s="56">
+        <v>1</v>
+      </c>
+      <c r="W30" s="56">
+        <v>2</v>
+      </c>
+      <c r="X30" s="56">
+        <v>3</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>335</v>
+      </c>
+      <c r="AO30" s="9"/>
+    </row>
+    <row r="31" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T31" s="17">
+        <v>0</v>
+      </c>
+      <c r="U31" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="V31" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="W31" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="X31" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y31" s="69"/>
+    </row>
+    <row r="32" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T32" s="17">
+        <v>1</v>
+      </c>
+      <c r="U32" s="48" t="s">
+        <v>317</v>
+      </c>
+      <c r="V32" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="W32" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y32" s="70"/>
+    </row>
+    <row r="33" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="17">
+        <v>2</v>
+      </c>
+      <c r="U33" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="V33" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="W33" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="X33" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y33" s="70"/>
+    </row>
+    <row r="34" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T34" s="17">
+        <v>3</v>
+      </c>
+      <c r="U34" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="V34" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="W34" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="X34" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y34" s="70"/>
+      <c r="AG34" s="9"/>
+      <c r="AH34" s="9"/>
+      <c r="AI34" s="9"/>
+      <c r="AJ34" s="9"/>
+      <c r="AK34" s="9"/>
+      <c r="AL34" s="9"/>
+      <c r="AM34" s="9"/>
+      <c r="AN34" s="9"/>
+      <c r="AO34" s="9"/>
+      <c r="AP34" s="9"/>
+      <c r="AQ34" s="9"/>
+      <c r="AR34" s="9"/>
+    </row>
+    <row r="35" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T35" s="17">
+        <v>4</v>
+      </c>
+      <c r="U35" s="89" t="s">
+        <v>320</v>
+      </c>
+      <c r="V35" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="W35" s="79" t="s">
+        <v>304</v>
+      </c>
+      <c r="X35" s="90" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y35" s="70"/>
+      <c r="AE35" s="18"/>
+      <c r="AF35" s="18"/>
+      <c r="AG35" s="13"/>
+      <c r="AH35" s="13"/>
+      <c r="AI35" s="13"/>
+      <c r="AJ35" s="13"/>
+      <c r="AK35" s="13"/>
+      <c r="AL35" s="13"/>
+      <c r="AM35" s="13"/>
+      <c r="AN35" s="13"/>
+      <c r="AO35" s="13"/>
+      <c r="AP35" s="13"/>
+      <c r="AQ35" s="13"/>
+      <c r="AR35" s="13"/>
+    </row>
+    <row r="36" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T36" s="17">
+        <v>5</v>
+      </c>
+      <c r="U36" s="91" t="s">
+        <v>321</v>
+      </c>
+      <c r="V36" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="W36" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="X36" s="92" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y36" s="70"/>
+      <c r="AE36" s="18"/>
+      <c r="AF36" s="18"/>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="13"/>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="13"/>
+      <c r="AM36" s="13"/>
+      <c r="AN36" s="13"/>
+      <c r="AO36" s="13"/>
+      <c r="AP36" s="13"/>
+      <c r="AQ36" s="13"/>
+      <c r="AR36" s="13"/>
+    </row>
+    <row r="37" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="17">
+        <v>6</v>
+      </c>
+      <c r="U37" s="91" t="s">
+        <v>322</v>
+      </c>
+      <c r="V37" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="W37" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="X37" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y37" s="70"/>
+      <c r="AE37" s="18"/>
+      <c r="AF37" s="18"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="13"/>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="13"/>
+      <c r="AL37" s="13"/>
+      <c r="AM37" s="13"/>
+      <c r="AN37" s="13"/>
+      <c r="AO37" s="13"/>
+      <c r="AP37" s="13"/>
+      <c r="AQ37" s="13"/>
+      <c r="AR37" s="13"/>
+    </row>
+    <row r="38" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T38" s="17">
+        <v>7</v>
+      </c>
+      <c r="U38" s="93" t="s">
+        <v>323</v>
+      </c>
+      <c r="V38" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="W38" s="94" t="s">
+        <v>307</v>
+      </c>
+      <c r="X38" s="95" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y38" s="65"/>
+      <c r="AE38" s="18"/>
+      <c r="AF38" s="18"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="13"/>
+      <c r="AM38" s="13"/>
+      <c r="AN38" s="13"/>
+      <c r="AO38" s="13"/>
+      <c r="AP38" s="13"/>
+      <c r="AQ38" s="13"/>
+      <c r="AR38" s="13"/>
+    </row>
+    <row r="39" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" display="https://juejin.cn/post/6844904063658639373"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add rotate to left 90
</commit_message>
<xml_diff>
--- a/tools/uv-工作簿1.xlsx
+++ b/tools/uv-工作簿1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 -copy (2)" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="视频尺寸" sheetId="3" r:id="rId3"/>
-    <sheet name="视频-blocks-转换--依据这个转换" sheetId="4" r:id="rId4"/>
+    <sheet name="视频-blocks右转90-转换--依据这个转换" sheetId="4" r:id="rId4"/>
+    <sheet name="视频-blocks左转90转换--依据这个转换" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="347">
   <si>
     <t>U0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1213,6 +1214,50 @@
   </si>
   <si>
     <t>NV12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rotate left 90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y98</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y114</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y121</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y122</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v26</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1325,15 +1370,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="50">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1834,6 +1915,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="5" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1843,7 +2001,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2133,6 +2291,141 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2144,6 +2437,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF339966"/>
       <color rgb="FF00FFCC"/>
     </mruColors>
   </colors>
@@ -2294,16 +2588,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>41275</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>130175</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:rowOff>187326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>147447</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71248</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2327,7 +2621,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000">
-          <a:off x="9686227" y="1731073"/>
+          <a:off x="11330877" y="1877124"/>
           <a:ext cx="4106672" cy="1616075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2594,6 +2888,357 @@
       <xdr:col>35</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
       <xdr:row>35</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9055100" y="6705600"/>
+          <a:ext cx="1841500" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>307976</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>73026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>165101</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>179198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="16200000">
+          <a:off x="11508678" y="1762824"/>
+          <a:ext cx="4106672" cy="1616075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>6351</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>208395</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="16200000">
+          <a:off x="14142028" y="1313873"/>
+          <a:ext cx="2551545" cy="1016000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 5" descr="YU12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="311150" y="6223000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 6" descr="YU12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="311150" y="6223000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="342900" y="6350000"/>
+          <a:ext cx="1841500" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 9" descr="NV12 Format"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9023350" y="7334250"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7048,8 +7693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -9091,4 +9736,2059 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AV45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ17" sqref="AJ17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="41" width="4.08203125" customWidth="1"/>
+    <col min="42" max="46" width="4.75" customWidth="1"/>
+    <col min="47" max="51" width="4.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20">
+        <v>3</v>
+      </c>
+      <c r="G2" s="20">
+        <v>4</v>
+      </c>
+      <c r="H2" s="20">
+        <v>5</v>
+      </c>
+      <c r="I2" s="20">
+        <v>6</v>
+      </c>
+      <c r="J2" s="20">
+        <v>7</v>
+      </c>
+      <c r="K2" s="20">
+        <v>8</v>
+      </c>
+      <c r="L2" s="20">
+        <v>9</v>
+      </c>
+      <c r="M2" s="20">
+        <v>10</v>
+      </c>
+      <c r="N2" s="20">
+        <v>11</v>
+      </c>
+      <c r="O2" s="20">
+        <v>12</v>
+      </c>
+      <c r="P2" s="20">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>14</v>
+      </c>
+      <c r="R2" s="20">
+        <v>15</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="U2" s="16">
+        <v>0</v>
+      </c>
+      <c r="V2" s="16">
+        <v>1</v>
+      </c>
+      <c r="W2" s="16">
+        <v>2</v>
+      </c>
+      <c r="X2" s="16">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="16">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="16">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="16">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="14"/>
+      <c r="AP2" t="s">
+        <v>336</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q3" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="R3" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" s="17">
+        <v>0</v>
+      </c>
+      <c r="U3" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="V3" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="W3" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="X3" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y3" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z3" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA3" s="79" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB3" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC3" s="66"/>
+    </row>
+    <row r="4" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="117" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="81" t="s">
+        <v>156</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="T4" s="17">
+        <v>1</v>
+      </c>
+      <c r="U4" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="V4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="W4" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y4" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA4" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB4" s="82" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC4" s="67"/>
+    </row>
+    <row r="5" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="20">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="R5" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="T5" s="17">
+        <v>2</v>
+      </c>
+      <c r="U5" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="W5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="X5" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA5" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB5" s="82" t="s">
+        <v>256</v>
+      </c>
+      <c r="AC5" s="67"/>
+    </row>
+    <row r="6" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="81" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="R6" s="82" t="s">
+        <v>193</v>
+      </c>
+      <c r="T6" s="17">
+        <v>3</v>
+      </c>
+      <c r="U6" s="81" t="s">
+        <v>147</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="W6" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="X6" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y6" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z6" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA6" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB6" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC6" s="67"/>
+    </row>
+    <row r="7" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="41">
+        <v>4</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="K7" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="R7" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="T7" s="17">
+        <v>4</v>
+      </c>
+      <c r="U7" s="81" t="s">
+        <v>146</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="W7" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="X7" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y7" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z7" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA7" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB7" s="82" t="s">
+        <v>254</v>
+      </c>
+      <c r="AC7" s="67"/>
+    </row>
+    <row r="8" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="41">
+        <v>5</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="R8" s="82" t="s">
+        <v>226</v>
+      </c>
+      <c r="T8" s="17">
+        <v>5</v>
+      </c>
+      <c r="U8" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="V8" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="W8" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="X8" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y8" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z8" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA8" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB8" s="82" t="s">
+        <v>343</v>
+      </c>
+      <c r="AC8" s="67"/>
+    </row>
+    <row r="9" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="41">
+        <v>6</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="K9" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="R9" s="82" t="s">
+        <v>242</v>
+      </c>
+      <c r="T9" s="17">
+        <v>6</v>
+      </c>
+      <c r="U9" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="W9" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="X9" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y9" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z9" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB9" s="82" t="s">
+        <v>342</v>
+      </c>
+      <c r="AC9" s="67"/>
+    </row>
+    <row r="10" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="41">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="K10" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="L10" s="84" t="s">
+        <v>252</v>
+      </c>
+      <c r="M10" s="84" t="s">
+        <v>253</v>
+      </c>
+      <c r="N10" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="O10" s="84" t="s">
+        <v>255</v>
+      </c>
+      <c r="P10" s="84" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q10" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="R10" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="T10" s="17">
+        <v>7</v>
+      </c>
+      <c r="U10" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="V10" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="W10" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="X10" s="84" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y10" s="84" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z10" s="84" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA10" s="84" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB10" s="85" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC10" s="67"/>
+    </row>
+    <row r="11" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="59"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="58"/>
+      <c r="T11" s="17">
+        <v>8</v>
+      </c>
+      <c r="U11" s="97" t="s">
+        <v>139</v>
+      </c>
+      <c r="V11" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="W11" s="79" t="s">
+        <v>169</v>
+      </c>
+      <c r="X11" s="79" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y11" s="79" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z11" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA11" s="79" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB11" s="98" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC11" s="67"/>
+    </row>
+    <row r="12" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="T12" s="17">
+        <v>9</v>
+      </c>
+      <c r="U12" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="V12" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="W12" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="X12" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y12" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z12" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA12" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="AB12" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC12" s="67"/>
+    </row>
+    <row r="13" spans="2:48" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>4</v>
+      </c>
+      <c r="H13" s="9">
+        <v>5</v>
+      </c>
+      <c r="I13" s="9">
+        <v>6</v>
+      </c>
+      <c r="J13" s="9">
+        <v>7</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="T13" s="17">
+        <v>10</v>
+      </c>
+      <c r="U13" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="V13" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="W13" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="X13" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y13" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z13" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA13" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB13" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC13" s="67"/>
+    </row>
+    <row r="14" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="18">
+        <v>0</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="H14" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="I14" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="T14" s="17">
+        <v>11</v>
+      </c>
+      <c r="U14" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="V14" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="W14" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="X14" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y14" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z14" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA14" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB14" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC14" s="67"/>
+    </row>
+    <row r="15" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>266</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="J15" s="75" t="s">
+        <v>269</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="T15" s="17">
+        <v>12</v>
+      </c>
+      <c r="U15" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="V15" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="W15" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="X15" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y15" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z15" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA15" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB15" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC15" s="67"/>
+    </row>
+    <row r="16" spans="2:48" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="G16" s="77" t="s">
+        <v>288</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="J16" s="75" t="s">
+        <v>291</v>
+      </c>
+      <c r="T16" s="17">
+        <v>13</v>
+      </c>
+      <c r="U16" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="V16" s="117" t="s">
+        <v>58</v>
+      </c>
+      <c r="W16" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="X16" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y16" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z16" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="AA16" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB16" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC16" s="67"/>
+    </row>
+    <row r="17" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="18">
+        <v>3</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="H17" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="I17" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="T17" s="17">
+        <v>14</v>
+      </c>
+      <c r="U17" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="W17" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="X17" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y17" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z17" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA17" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB17" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC17" s="67"/>
+    </row>
+    <row r="18" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="18"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
+      <c r="T18" s="17">
+        <v>15</v>
+      </c>
+      <c r="U18" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="W18" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="X18" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y18" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z18" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA18" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB18" s="99" t="s">
+        <v>243</v>
+      </c>
+      <c r="AC18" s="68"/>
+    </row>
+    <row r="19" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>3</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4</v>
+      </c>
+      <c r="H20" s="11">
+        <v>5</v>
+      </c>
+      <c r="I20" s="11">
+        <v>6</v>
+      </c>
+      <c r="J20" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="18">
+        <v>0</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="86" t="s">
+        <v>298</v>
+      </c>
+      <c r="H21" s="87" t="s">
+        <v>299</v>
+      </c>
+      <c r="I21" s="87" t="s">
+        <v>300</v>
+      </c>
+      <c r="J21" s="88" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18">
+        <v>1</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="G22" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="J22" s="75" t="s">
+        <v>307</v>
+      </c>
+      <c r="AO22" s="16"/>
+    </row>
+    <row r="23" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18">
+        <v>2</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="G23" s="77" t="s">
+        <v>312</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="J23" s="75" t="s">
+        <v>315</v>
+      </c>
+      <c r="AO23" s="25"/>
+    </row>
+    <row r="24" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="18">
+        <v>3</v>
+      </c>
+      <c r="C24" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="F24" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="H24" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO24" s="25"/>
+    </row>
+    <row r="25" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="65"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AF25" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="AO25" s="25"/>
+    </row>
+    <row r="26" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S26" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="T26" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="U26" s="16">
+        <v>0</v>
+      </c>
+      <c r="V26" s="16">
+        <v>1</v>
+      </c>
+      <c r="W26" s="16">
+        <v>2</v>
+      </c>
+      <c r="X26" s="16">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE26" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="56">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="16">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="56">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="16">
+        <v>2</v>
+      </c>
+      <c r="AJ26" s="56">
+        <v>2</v>
+      </c>
+      <c r="AK26" s="16">
+        <v>3</v>
+      </c>
+      <c r="AL26" s="56">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="25"/>
+    </row>
+    <row r="27" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>333</v>
+      </c>
+      <c r="T27" s="17">
+        <v>0</v>
+      </c>
+      <c r="U27" s="113" t="s">
+        <v>263</v>
+      </c>
+      <c r="V27" s="114" t="s">
+        <v>269</v>
+      </c>
+      <c r="W27" s="114" t="s">
+        <v>277</v>
+      </c>
+      <c r="X27" s="115" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y27" s="69"/>
+      <c r="AD27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="116" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF27" s="107" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG27" s="117" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH27" s="107" t="s">
+        <v>307</v>
+      </c>
+      <c r="AI27" s="117" t="s">
+        <v>277</v>
+      </c>
+      <c r="AJ27" s="107" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK27" s="117" t="s">
+        <v>285</v>
+      </c>
+      <c r="AL27" s="108" t="s">
+        <v>323</v>
+      </c>
+      <c r="AM27" s="71"/>
+      <c r="AO27" s="9"/>
+    </row>
+    <row r="28" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="55" t="s">
+        <v>334</v>
+      </c>
+      <c r="T28" s="17">
+        <v>1</v>
+      </c>
+      <c r="U28" s="116" t="s">
+        <v>262</v>
+      </c>
+      <c r="V28" s="117" t="s">
+        <v>268</v>
+      </c>
+      <c r="W28" s="117" t="s">
+        <v>276</v>
+      </c>
+      <c r="X28" s="118" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y28" s="67"/>
+      <c r="AD28" s="17">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="116" t="s">
+        <v>262</v>
+      </c>
+      <c r="AF28" s="107" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG28" s="117" t="s">
+        <v>268</v>
+      </c>
+      <c r="AH28" s="107" t="s">
+        <v>306</v>
+      </c>
+      <c r="AI28" s="117" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ28" s="107" t="s">
+        <v>314</v>
+      </c>
+      <c r="AK28" s="117" t="s">
+        <v>284</v>
+      </c>
+      <c r="AL28" s="108" t="s">
+        <v>322</v>
+      </c>
+      <c r="AM28" s="72"/>
+      <c r="AO28" s="9"/>
+    </row>
+    <row r="29" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T29" s="17">
+        <v>2</v>
+      </c>
+      <c r="U29" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="V29" s="117" t="s">
+        <v>267</v>
+      </c>
+      <c r="W29" s="117" t="s">
+        <v>275</v>
+      </c>
+      <c r="X29" s="118" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y29" s="70"/>
+      <c r="AD29" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE29" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF29" s="107" t="s">
+        <v>299</v>
+      </c>
+      <c r="AG29" s="117" t="s">
+        <v>267</v>
+      </c>
+      <c r="AH29" s="107" t="s">
+        <v>305</v>
+      </c>
+      <c r="AI29" s="117" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ29" s="107" t="s">
+        <v>313</v>
+      </c>
+      <c r="AK29" s="117" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL29" s="108" t="s">
+        <v>321</v>
+      </c>
+      <c r="AM29" s="72"/>
+      <c r="AO29" s="9"/>
+    </row>
+    <row r="30" spans="2:41" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T30" s="17">
+        <v>3</v>
+      </c>
+      <c r="U30" s="119" t="s">
+        <v>260</v>
+      </c>
+      <c r="V30" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="W30" s="120" t="s">
+        <v>274</v>
+      </c>
+      <c r="X30" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y30" s="70"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="17">
+        <v>3</v>
+      </c>
+      <c r="AE30" s="116" t="s">
+        <v>260</v>
+      </c>
+      <c r="AF30" s="107" t="s">
+        <v>298</v>
+      </c>
+      <c r="AG30" s="117" t="s">
+        <v>266</v>
+      </c>
+      <c r="AH30" s="107" t="s">
+        <v>304</v>
+      </c>
+      <c r="AI30" s="117" t="s">
+        <v>274</v>
+      </c>
+      <c r="AJ30" s="107" t="s">
+        <v>312</v>
+      </c>
+      <c r="AK30" s="117" t="s">
+        <v>282</v>
+      </c>
+      <c r="AL30" s="108" t="s">
+        <v>320</v>
+      </c>
+      <c r="AM30" s="72"/>
+      <c r="AO30" s="9"/>
+    </row>
+    <row r="31" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T31" s="17">
+        <v>4</v>
+      </c>
+      <c r="U31" s="122" t="s">
+        <v>259</v>
+      </c>
+      <c r="V31" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="W31" s="110" t="s">
+        <v>273</v>
+      </c>
+      <c r="X31" s="123" t="s">
+        <v>281</v>
+      </c>
+      <c r="Y31" s="70"/>
+      <c r="AD31" s="17">
+        <v>4</v>
+      </c>
+      <c r="AE31" s="109" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF31" s="138" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG31" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="AH31" s="138" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI31" s="110" t="s">
+        <v>273</v>
+      </c>
+      <c r="AJ31" s="138" t="s">
+        <v>311</v>
+      </c>
+      <c r="AK31" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL31" s="140" t="s">
+        <v>319</v>
+      </c>
+      <c r="AM31" s="72"/>
+    </row>
+    <row r="32" spans="2:41" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T32" s="17">
+        <v>5</v>
+      </c>
+      <c r="U32" s="122" t="s">
+        <v>24</v>
+      </c>
+      <c r="V32" s="110" t="s">
+        <v>344</v>
+      </c>
+      <c r="W32" s="110" t="s">
+        <v>286</v>
+      </c>
+      <c r="X32" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y32" s="70"/>
+      <c r="AD32" s="17">
+        <v>5</v>
+      </c>
+      <c r="AE32" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF32" s="138" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG32" s="110" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH32" s="138" t="s">
+        <v>330</v>
+      </c>
+      <c r="AI32" s="110" t="s">
+        <v>286</v>
+      </c>
+      <c r="AJ32" s="138" t="s">
+        <v>345</v>
+      </c>
+      <c r="AK32" s="110" t="s">
+        <v>292</v>
+      </c>
+      <c r="AL32" s="140" t="s">
+        <v>346</v>
+      </c>
+      <c r="AM32" s="72"/>
+    </row>
+    <row r="33" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="17">
+        <v>6</v>
+      </c>
+      <c r="U33" s="122" t="s">
+        <v>22</v>
+      </c>
+      <c r="V33" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="W33" s="110" t="s">
+        <v>271</v>
+      </c>
+      <c r="X33" s="123" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y33" s="70"/>
+      <c r="AD33" s="17">
+        <v>6</v>
+      </c>
+      <c r="AE33" s="109" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF33" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG33" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH33" s="138" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI33" s="110" t="s">
+        <v>271</v>
+      </c>
+      <c r="AJ33" s="138" t="s">
+        <v>309</v>
+      </c>
+      <c r="AK33" s="110" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL33" s="140" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM33" s="72"/>
+    </row>
+    <row r="34" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T34" s="17">
+        <v>7</v>
+      </c>
+      <c r="U34" s="124" t="s">
+        <v>20</v>
+      </c>
+      <c r="V34" s="125" t="s">
+        <v>36</v>
+      </c>
+      <c r="W34" s="125" t="s">
+        <v>270</v>
+      </c>
+      <c r="X34" s="126" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y34" s="65"/>
+      <c r="AD34" s="17">
+        <v>7</v>
+      </c>
+      <c r="AE34" s="111" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF34" s="139" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG34" s="112" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH34" s="139" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI34" s="112" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ34" s="139" t="s">
+        <v>308</v>
+      </c>
+      <c r="AK34" s="112" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL34" s="141" t="s">
+        <v>316</v>
+      </c>
+      <c r="AM34" s="73"/>
+      <c r="AN34" s="9"/>
+      <c r="AO34" s="9"/>
+      <c r="AP34" s="9"/>
+      <c r="AQ34" s="9"/>
+      <c r="AR34" s="9"/>
+    </row>
+    <row r="35" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AN35" s="13"/>
+      <c r="AO35" s="13"/>
+      <c r="AP35" s="13"/>
+      <c r="AQ35" s="13"/>
+      <c r="AR35" s="13"/>
+    </row>
+    <row r="36" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T36" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="U36" s="56">
+        <v>0</v>
+      </c>
+      <c r="V36" s="56">
+        <v>1</v>
+      </c>
+      <c r="W36" s="56">
+        <v>2</v>
+      </c>
+      <c r="X36" s="56">
+        <v>3</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>335</v>
+      </c>
+      <c r="AN36" s="13"/>
+      <c r="AO36" s="13"/>
+      <c r="AP36" s="13"/>
+      <c r="AQ36" s="13"/>
+      <c r="AR36" s="13"/>
+    </row>
+    <row r="37" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="17">
+        <v>0</v>
+      </c>
+      <c r="U37" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="V37" s="102" t="s">
+        <v>307</v>
+      </c>
+      <c r="W37" s="102" t="s">
+        <v>315</v>
+      </c>
+      <c r="X37" s="103" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y37" s="69"/>
+      <c r="AN37" s="13"/>
+      <c r="AO37" s="13"/>
+      <c r="AP37" s="13"/>
+      <c r="AQ37" s="13"/>
+      <c r="AR37" s="13"/>
+    </row>
+    <row r="38" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T38" s="17">
+        <v>1</v>
+      </c>
+      <c r="U38" s="104" t="s">
+        <v>300</v>
+      </c>
+      <c r="V38" s="105" t="s">
+        <v>306</v>
+      </c>
+      <c r="W38" s="105" t="s">
+        <v>314</v>
+      </c>
+      <c r="X38" s="106" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y38" s="70"/>
+      <c r="AN38" s="13"/>
+      <c r="AO38" s="13"/>
+      <c r="AP38" s="13"/>
+      <c r="AQ38" s="13"/>
+      <c r="AR38" s="13"/>
+    </row>
+    <row r="39" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T39" s="17">
+        <v>2</v>
+      </c>
+      <c r="U39" s="104" t="s">
+        <v>299</v>
+      </c>
+      <c r="V39" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="W39" s="105" t="s">
+        <v>313</v>
+      </c>
+      <c r="X39" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y39" s="70"/>
+    </row>
+    <row r="40" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T40" s="17">
+        <v>3</v>
+      </c>
+      <c r="U40" s="127" t="s">
+        <v>298</v>
+      </c>
+      <c r="V40" s="128" t="s">
+        <v>304</v>
+      </c>
+      <c r="W40" s="128" t="s">
+        <v>312</v>
+      </c>
+      <c r="X40" s="129" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y40" s="70"/>
+      <c r="AG40" s="9"/>
+      <c r="AH40" s="9"/>
+      <c r="AI40" s="9"/>
+      <c r="AJ40" s="9"/>
+      <c r="AK40" s="9"/>
+      <c r="AL40" s="9"/>
+      <c r="AM40" s="9"/>
+    </row>
+    <row r="41" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T41" s="17">
+        <v>4</v>
+      </c>
+      <c r="U41" s="130" t="s">
+        <v>137</v>
+      </c>
+      <c r="V41" s="131" t="s">
+        <v>303</v>
+      </c>
+      <c r="W41" s="131" t="s">
+        <v>311</v>
+      </c>
+      <c r="X41" s="132" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y41" s="70"/>
+      <c r="AE41" s="18"/>
+      <c r="AF41" s="18"/>
+      <c r="AG41" s="13"/>
+      <c r="AH41" s="13"/>
+      <c r="AI41" s="13"/>
+      <c r="AJ41" s="13"/>
+      <c r="AK41" s="13"/>
+      <c r="AL41" s="13"/>
+      <c r="AM41" s="13"/>
+    </row>
+    <row r="42" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T42" s="17">
+        <v>5</v>
+      </c>
+      <c r="U42" s="133" t="s">
+        <v>25</v>
+      </c>
+      <c r="V42" s="100" t="s">
+        <v>330</v>
+      </c>
+      <c r="W42" s="100" t="s">
+        <v>345</v>
+      </c>
+      <c r="X42" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="Y42" s="70"/>
+      <c r="AE42" s="18"/>
+      <c r="AF42" s="18"/>
+      <c r="AG42" s="13"/>
+      <c r="AH42" s="13"/>
+      <c r="AI42" s="13"/>
+      <c r="AJ42" s="13"/>
+      <c r="AK42" s="13"/>
+      <c r="AL42" s="13"/>
+      <c r="AM42" s="13"/>
+    </row>
+    <row r="43" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T43" s="17">
+        <v>6</v>
+      </c>
+      <c r="U43" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="V43" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="W43" s="100" t="s">
+        <v>309</v>
+      </c>
+      <c r="X43" s="134" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y43" s="70"/>
+      <c r="AE43" s="18"/>
+      <c r="AF43" s="18"/>
+      <c r="AG43" s="13"/>
+      <c r="AH43" s="13"/>
+      <c r="AI43" s="13"/>
+      <c r="AJ43" s="13"/>
+      <c r="AK43" s="13"/>
+      <c r="AL43" s="13"/>
+      <c r="AM43" s="13"/>
+    </row>
+    <row r="44" spans="20:44" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T44" s="17">
+        <v>7</v>
+      </c>
+      <c r="U44" s="135" t="s">
+        <v>21</v>
+      </c>
+      <c r="V44" s="136" t="s">
+        <v>37</v>
+      </c>
+      <c r="W44" s="136" t="s">
+        <v>308</v>
+      </c>
+      <c r="X44" s="137" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y44" s="65"/>
+      <c r="AE44" s="18"/>
+      <c r="AF44" s="18"/>
+      <c r="AG44" s="13"/>
+      <c r="AH44" s="13"/>
+      <c r="AI44" s="13"/>
+      <c r="AJ44" s="13"/>
+      <c r="AK44" s="13"/>
+      <c r="AL44" s="13"/>
+      <c r="AM44" s="13"/>
+    </row>
+    <row r="45" spans="20:44" ht="17.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" display="https://juejin.cn/post/6844904063658639373"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>